<commit_message>
Setting tab TC-01,02 added (27/10/25)
</commit_message>
<xml_diff>
--- a/testData/SettingTestCaseTestData/settingTab_testData.xlsx
+++ b/testData/SettingTestCaseTestData/settingTab_testData.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MohitAman\Desktop\UAT_NEXTNEXT_BLAZE_FRAMEWORK_AUTO\testData\SettingTestCaseTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99AB18F4-7D25-42D3-9599-AB9369C42820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED615B3-CE72-4238-AEEB-6E9112736DBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demo" sheetId="2" r:id="rId1"/>
     <sheet name="Demo1" sheetId="3" r:id="rId2"/>
+    <sheet name="tc002" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t>Fieldvalue</t>
   </si>
@@ -86,6 +87,24 @@
   </si>
   <si>
     <t>check</t>
+  </si>
+  <si>
+    <t>fieldName</t>
+  </si>
+  <si>
+    <t>textBox</t>
+  </si>
+  <si>
+    <t>objType1</t>
+  </si>
+  <si>
+    <t>objType2</t>
+  </si>
+  <si>
+    <t>Req</t>
+  </si>
+  <si>
+    <t>Test Cases</t>
   </si>
 </sst>
 </file>
@@ -121,8 +140,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,7 +507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{893CB98F-CAE6-4140-81F6-9A9E84844E60}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -528,4 +550,53 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B7CF4F0-0715-4424-A70F-25AC2557DEA6}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="12.7265625" customWidth="1"/>
+    <col min="3" max="3" width="15.26953125" customWidth="1"/>
+    <col min="4" max="4" width="15.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Setting tab TC-01,02,09 added (27/10/25)
</commit_message>
<xml_diff>
--- a/testData/SettingTestCaseTestData/settingTab_testData.xlsx
+++ b/testData/SettingTestCaseTestData/settingTab_testData.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MohitAman\Desktop\UAT_NEXTNEXT_BLAZE_FRAMEWORK_AUTO\testData\SettingTestCaseTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED615B3-CE72-4238-AEEB-6E9112736DBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A63A732-9A9F-4F60-AC6B-9B2A7E04C1A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demo" sheetId="2" r:id="rId1"/>
     <sheet name="Demo1" sheetId="3" r:id="rId2"/>
     <sheet name="tc002" sheetId="4" r:id="rId3"/>
+    <sheet name="tc009" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
   <si>
     <t>Fieldvalue</t>
   </si>
@@ -105,6 +106,12 @@
   </si>
   <si>
     <t>Test Cases</t>
+  </si>
+  <si>
+    <t>fieldname</t>
+  </si>
+  <si>
+    <t>Category</t>
   </si>
 </sst>
 </file>
@@ -556,7 +563,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B7CF4F0-0715-4424-A70F-25AC2557DEA6}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -599,4 +606,35 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA67621A-69E9-473D-A7D8-F9F0F26841F1}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Dont merge this in main
</commit_message>
<xml_diff>
--- a/testData/SettingTestCaseTestData/settingTab_testData.xlsx
+++ b/testData/SettingTestCaseTestData/settingTab_testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MohitAman\Desktop\UAT_NEXTNEXT_BLAZE_FRAMEWORK_AUTO\testData\SettingTestCaseTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{672645E2-E6EF-4507-90FD-B025E5451F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF275E84-9285-43A4-98DC-6A638E79AADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demo" sheetId="2" r:id="rId1"/>
@@ -20,6 +20,9 @@
     <sheet name="tc015" sheetId="7" r:id="rId5"/>
     <sheet name="tc016" sheetId="8" r:id="rId6"/>
     <sheet name="tc010" sheetId="6" r:id="rId7"/>
+    <sheet name="tc022" sheetId="9" r:id="rId8"/>
+    <sheet name="tc023" sheetId="10" r:id="rId9"/>
+    <sheet name="tc028" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="33">
   <si>
     <t>Fieldvalue</t>
   </si>
@@ -121,6 +124,15 @@
   </si>
   <si>
     <t>def_value</t>
+  </si>
+  <si>
+    <t>New Rq</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>text</t>
   </si>
 </sst>
 </file>
@@ -519,6 +531,37 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13D55113-FCD4-4302-ACCC-5A1231CFD9C3}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{893CB98F-CAE6-4140-81F6-9A9E84844E60}">
   <dimension ref="A1:D2"/>
@@ -683,7 +726,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D2B50D4-23AC-45FA-9C3E-A69469D94C96}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -742,4 +785,75 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5098D96-EDBC-47E2-A3DC-EA160990E15F}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0580A98-7D2C-4174-84B3-26733BA04D97}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>